<commit_message>
Improved spreadsheet for bulk loaded announcements. Updated announcements columns in bulk edit page to match new requirements.
</commit_message>
<xml_diff>
--- a/test/unit/resources/announcements.xlsx
+++ b/test/unit/resources/announcements.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="25360" windowHeight="13560"/>
+    <workbookView xWindow="28320" yWindow="2600" windowWidth="25360" windowHeight="13560"/>
   </bookViews>
   <sheets>
     <sheet name="Announcements" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Grant ID</t>
   </si>
@@ -27,21 +27,6 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Proposed event/announcement</t>
-  </si>
-  <si>
-    <t>Proposed Date of event / announcement (if known)</t>
-  </si>
-  <si>
-    <t>Type of event / announcement (if known)</t>
-  </si>
-  <si>
-    <t>Description of the event</t>
-  </si>
-  <si>
-    <t>Value of the funding round</t>
-  </si>
-  <si>
     <t>Grant 0</t>
   </si>
   <si>
@@ -51,12 +36,6 @@
     <t>Event 0</t>
   </si>
   <si>
-    <t>2015-06-00</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Description 0</t>
   </si>
   <si>
@@ -69,9 +48,6 @@
     <t>Event 1</t>
   </si>
   <si>
-    <t>2015-06-01</t>
-  </si>
-  <si>
     <t>Description 1</t>
   </si>
   <si>
@@ -84,9 +60,6 @@
     <t>Event 2</t>
   </si>
   <si>
-    <t>2015-06-02</t>
-  </si>
-  <si>
     <t>Description 2</t>
   </si>
   <si>
@@ -99,9 +72,6 @@
     <t>Event 3</t>
   </si>
   <si>
-    <t>2015-06-03</t>
-  </si>
-  <si>
     <t>Description 3</t>
   </si>
   <si>
@@ -114,9 +84,6 @@
     <t>Event 4</t>
   </si>
   <si>
-    <t>2015-06-04</t>
-  </si>
-  <si>
     <t>Description 4</t>
   </si>
   <si>
@@ -129,9 +96,6 @@
     <t>Event 5</t>
   </si>
   <si>
-    <t>2015-06-05</t>
-  </si>
-  <si>
     <t>Description 5</t>
   </si>
   <si>
@@ -144,9 +108,6 @@
     <t>Event 6</t>
   </si>
   <si>
-    <t>2015-06-06</t>
-  </si>
-  <si>
     <t>Description 6</t>
   </si>
   <si>
@@ -159,9 +120,6 @@
     <t>Event 7</t>
   </si>
   <si>
-    <t>2015-06-07</t>
-  </si>
-  <si>
     <t>Description 7</t>
   </si>
   <si>
@@ -174,9 +132,6 @@
     <t>Event 8</t>
   </si>
   <si>
-    <t>2015-06-08</t>
-  </si>
-  <si>
     <t>Description 8</t>
   </si>
   <si>
@@ -189,20 +144,57 @@
     <t>Event 9</t>
   </si>
   <si>
-    <t>2015-06-09</t>
-  </si>
-  <si>
     <t>Description 9</t>
+  </si>
+  <si>
+    <t>Name of Grant round or non-funding op</t>
+  </si>
+  <si>
+    <t>Scheduled date for grant round opening of other non-funding opp</t>
+  </si>
+  <si>
+    <t>Total value of grant round</t>
+  </si>
+  <si>
+    <t>Information about this grant round or non-funding op</t>
+  </si>
+  <si>
+    <t>When will these grants be announced</t>
+  </si>
+  <si>
+    <t>Type of event / announcement</t>
+  </si>
+  <si>
+    <t>Non-funding op</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,13 +217,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,13 +566,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,253 +586,285 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D2" s="1">
+        <v>42156</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" s="1">
+        <v>42005</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" s="1">
+        <v>42157</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G3" s="1">
+        <v>42037</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="D4" s="1">
+        <v>42158</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D5" s="1">
+        <v>42159</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="G5" s="1">
+        <v>42098</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" s="1">
+        <v>42160</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G6" s="1">
+        <v>42129</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D7" s="1">
+        <v>42161</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G7" s="1">
+        <v>42161</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D8" s="1">
+        <v>42162</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G8" s="1">
+        <v>42192</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="D9" s="1">
+        <v>42163</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G9" s="1">
+        <v>42224</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D10" s="1">
+        <v>42164</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
         <v>37</v>
       </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="G10" s="1">
+        <v>42256</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D11" s="1">
+        <v>42165</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11">
-        <v>9</v>
+      <c r="G11" s="1">
+        <v>42287</v>
+      </c>
+      <c r="H11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Renamed / reordered columns per latest announcements changes.
</commit_message>
<xml_diff>
--- a/test/unit/resources/announcements.xlsx
+++ b/test/unit/resources/announcements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28320" yWindow="2600" windowWidth="25360" windowHeight="13560"/>
+    <workbookView xWindow="2680" yWindow="2860" windowWidth="25360" windowHeight="13580"/>
   </bookViews>
   <sheets>
     <sheet name="Announcements" sheetId="1" r:id="rId1"/>
@@ -147,25 +147,25 @@
     <t>Description 9</t>
   </si>
   <si>
-    <t>Name of Grant round or non-funding op</t>
-  </si>
-  <si>
-    <t>Scheduled date for grant round opening of other non-funding opp</t>
-  </si>
-  <si>
-    <t>Total value of grant round</t>
-  </si>
-  <si>
-    <t>Information about this grant round or non-funding op</t>
-  </si>
-  <si>
-    <t>When will these grants be announced</t>
-  </si>
-  <si>
-    <t>Type of event / announcement</t>
-  </si>
-  <si>
     <t>Non-funding op</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Name of funding announcement or non-funding opportunity</t>
+  </si>
+  <si>
+    <t>Scheduled date for: 1 - Announcing the opening of the grant round; 2 - Non-funding opportunities</t>
+  </si>
+  <si>
+    <t>When will successful applicants be announced</t>
+  </si>
+  <si>
+    <t>Total value of funding announcement</t>
+  </si>
+  <si>
+    <t>Information about this funding announcement or non-funding opportunity</t>
   </si>
 </sst>
 </file>
@@ -217,8 +217,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -230,13 +234,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,13 +577,14 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -586,22 +595,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -612,22 +621,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>42156</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="1">
+        <v>42005</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>42005</v>
-      </c>
-      <c r="H2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -638,22 +647,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>42157</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="1">
+        <v>42037</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c r="G3" s="1">
-        <v>42037</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -664,20 +673,20 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>42158</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="1"/>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -688,22 +697,22 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>42159</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="1">
+        <v>42098</v>
+      </c>
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
-      </c>
-      <c r="G5" s="1">
-        <v>42098</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -714,22 +723,22 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>42160</v>
       </c>
-      <c r="E6">
+      <c r="F6" s="1">
+        <v>42129</v>
+      </c>
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" s="1">
-        <v>42129</v>
-      </c>
-      <c r="H6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -740,22 +749,22 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>42161</v>
       </c>
-      <c r="E7">
+      <c r="F7" s="1">
+        <v>42161</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>25</v>
-      </c>
-      <c r="G7" s="1">
-        <v>42161</v>
-      </c>
-      <c r="H7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -766,22 +775,22 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>42162</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="1">
+        <v>42192</v>
+      </c>
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>29</v>
-      </c>
-      <c r="G8" s="1">
-        <v>42192</v>
-      </c>
-      <c r="H8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -792,22 +801,22 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>42163</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="1">
+        <v>42224</v>
+      </c>
+      <c r="G9">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>33</v>
-      </c>
-      <c r="G9" s="1">
-        <v>42224</v>
-      </c>
-      <c r="H9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -818,22 +827,22 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>42164</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="1">
+        <v>42256</v>
+      </c>
+      <c r="G10">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" s="1">
-        <v>42256</v>
-      </c>
-      <c r="H10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -844,22 +853,22 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>42165</v>
       </c>
-      <c r="E11">
+      <c r="F11" s="1">
+        <v>42287</v>
+      </c>
+      <c r="G11">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>41</v>
-      </c>
-      <c r="G11" s="1">
-        <v>42287</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>